<commit_message>
Isuue | #263 | ajuste de carga masiva
</commit_message>
<xml_diff>
--- a/public/formats/co-documents-batch.xlsx
+++ b/public/formats/co-documents-batch.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\facturador_co\public\formats\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9210"/>
   </bookViews>
   <sheets>
     <sheet name="Document" sheetId="1" r:id="rId1"/>
@@ -16,8 +21,8 @@
     <definedName name="CodigoMetodoPago">'Código metodo de pago'!$B$2:$B$76</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -30,7 +35,7 @@
     <author>USER</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -78,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -126,7 +131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -150,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -174,7 +179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -198,7 +203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -222,7 +227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -246,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -270,7 +275,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -294,7 +299,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -318,7 +323,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -342,7 +347,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -366,7 +371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -390,7 +395,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -414,7 +419,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="Q1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -438,7 +443,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -462,7 +467,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0">
+    <comment ref="S1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -486,7 +491,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0">
+    <comment ref="T1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -510,7 +515,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="U1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -534,7 +539,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0">
+    <comment ref="V1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -558,7 +563,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0">
+    <comment ref="W1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -582,7 +587,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="X1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -606,7 +611,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0">
+    <comment ref="Y1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -630,7 +635,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0">
+    <comment ref="Z1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -654,7 +659,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0">
+    <comment ref="AA1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -678,7 +683,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0">
+    <comment ref="AB1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -702,7 +707,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0">
+    <comment ref="AC1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -726,7 +731,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0">
+    <comment ref="AD1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -750,7 +755,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0">
+    <comment ref="AE1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -809,7 +814,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="141">
   <si>
     <t>Periodo facturacion Junio 2023</t>
   </si>
@@ -820,399 +825,429 @@
     <t>presidente@ipsnelsonmandela.com</t>
   </si>
   <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>FUNDACION CLINICA NELSON MANDELA, Amor por servir</t>
+  </si>
+  <si>
+    <t>Calle 102 No. 24a 15, Barrio Compartir, Cali, Valle del Cauca - 602 389 9301 - www.ipsnelsonmandela.com</t>
+  </si>
+  <si>
+    <t>CALLE 102 No. 24A-15</t>
+  </si>
+  <si>
+    <t>18760000001</t>
+  </si>
+  <si>
+    <t>SETP</t>
+  </si>
+  <si>
+    <t>PRUEBA2</t>
+  </si>
+  <si>
+    <t>numero</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>hora</t>
+  </si>
+  <si>
+    <t>numero_resolucion</t>
+  </si>
+  <si>
+    <t>prefijo</t>
+  </si>
+  <si>
+    <t>nombre_establecimiento</t>
+  </si>
+  <si>
+    <t>direccion_establecimiento</t>
+  </si>
+  <si>
+    <t>telefono_establecimiento</t>
+  </si>
+  <si>
+    <t>municipio_establecimiento</t>
+  </si>
+  <si>
+    <t>email_establecimiento</t>
+  </si>
+  <si>
+    <t>idetificacion_cliente</t>
+  </si>
+  <si>
+    <t>id_forma_pago</t>
+  </si>
+  <si>
+    <t>id_metodo_pago</t>
+  </si>
+  <si>
+    <t>fecha_vencimiento</t>
+  </si>
+  <si>
+    <t>plazo_dias</t>
+  </si>
+  <si>
+    <t>total_impuestos_incl</t>
+  </si>
+  <si>
+    <t>total_descuentos</t>
+  </si>
+  <si>
+    <t>total_cargos</t>
+  </si>
+  <si>
+    <t>total_pagado</t>
+  </si>
+  <si>
+    <t>cantidad_linea</t>
+  </si>
+  <si>
+    <t>base_impuestos_linea</t>
+  </si>
+  <si>
+    <t>codigo_linea</t>
+  </si>
+  <si>
+    <t>precio_venta</t>
+  </si>
+  <si>
+    <t>nota_cabecera</t>
+  </si>
+  <si>
+    <t>nota_pie</t>
+  </si>
+  <si>
+    <t>notas_factura</t>
+  </si>
+  <si>
+    <t>fecha_inicial_perido_facturado</t>
+  </si>
+  <si>
+    <t>fecha_final_perido_facturado</t>
+  </si>
+  <si>
+    <t>informacion_usuarios_sector_salud</t>
+  </si>
+  <si>
+    <t>total_base_impuestos</t>
+  </si>
+  <si>
+    <t>total_valor_bruto</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Contado</t>
+  </si>
+  <si>
+    <t>Crédito</t>
+  </si>
+  <si>
+    <t>Instrumento no definido</t>
+  </si>
+  <si>
+    <t>Crédito ACH</t>
+  </si>
+  <si>
+    <t>Débito ACH</t>
+  </si>
+  <si>
+    <t>Reversión débito de demanda ACH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reversión crédito de demanda ACH </t>
+  </si>
+  <si>
+    <t>Crédito de demanda ACH</t>
+  </si>
+  <si>
+    <t>Débito de demanda ACH</t>
+  </si>
+  <si>
+    <t>Mantener</t>
+  </si>
+  <si>
+    <t>Clearing Nacional o Regional</t>
+  </si>
+  <si>
+    <t>Efectivo</t>
+  </si>
+  <si>
+    <t>Reversión Crédito Ahorro</t>
+  </si>
+  <si>
+    <t>Reversión Débito Ahorro</t>
+  </si>
+  <si>
+    <t>Crédito Ahorro</t>
+  </si>
+  <si>
+    <t>Débito Ahorro</t>
+  </si>
+  <si>
+    <t>Bookentry Crédito</t>
+  </si>
+  <si>
+    <t>Bookentry Débito</t>
+  </si>
+  <si>
+    <t>Concentración de la demanda en efectivo /Desembolso Crédito (CCD)</t>
+  </si>
+  <si>
+    <t>Concentración de la demanda en efectivo / Desembolso (CCD) débito</t>
+  </si>
+  <si>
+    <t>Crédito Pago negocio corporativo (CTP)</t>
+  </si>
+  <si>
+    <t>Cheque</t>
+  </si>
+  <si>
+    <t>Poyecto bancario</t>
+  </si>
+  <si>
+    <t>Proyecto bancario certificado</t>
+  </si>
+  <si>
+    <t>Cheque bancario</t>
+  </si>
+  <si>
+    <t>Nota cambiaria esperando aceptación</t>
+  </si>
+  <si>
+    <t>Cheque certificado</t>
+  </si>
+  <si>
+    <t>Cheque Local</t>
+  </si>
+  <si>
+    <t>Débito Pago Neogcio Corporativo (CTP)</t>
+  </si>
+  <si>
+    <t>Crédito Negocio Intercambio Corporativo (CTX)</t>
+  </si>
+  <si>
+    <t>Débito Negocio Intercambio Corporativo (CTX)</t>
+  </si>
+  <si>
+    <t>Transferecia Crédito</t>
+  </si>
+  <si>
+    <t>Transferencia Débito</t>
+  </si>
+  <si>
+    <t>Concentración Efectivo / Desembolso Crédito plus (CCD+)</t>
+  </si>
+  <si>
+    <t>Concentración Efectivo / Desembolso Débito plus (CCD+)</t>
+  </si>
+  <si>
+    <t>Pago y depósito pre acordado (PPD)</t>
+  </si>
+  <si>
+    <t>Concentración efectivo ahorros / Desembolso Crédito (CCD)</t>
+  </si>
+  <si>
+    <t>Concentración efectivo ahorros / Desembolso Drédito (CCD)</t>
+  </si>
+  <si>
+    <t>Pago Negocio Corporativo Ahorros Crédito (CTP)</t>
+  </si>
+  <si>
+    <t>Pago Neogcio Corporativo Ahorros Débito (CTP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Concentración efectivo/Desembolso Crédito plus (CCD+) </t>
+  </si>
+  <si>
+    <t>Consiganción bancaria</t>
+  </si>
+  <si>
+    <t>Concentración efectivo / Desembolso Débito plus (CCD+)</t>
+  </si>
+  <si>
+    <t>Nota cambiaria</t>
+  </si>
+  <si>
+    <t>Transferencia Crédito Bancario</t>
+  </si>
+  <si>
+    <t>Transferencia Débito Interbancario</t>
+  </si>
+  <si>
+    <t>Transferencia Débito Bancaria</t>
+  </si>
+  <si>
+    <t>Tarjeta Crédito</t>
+  </si>
+  <si>
+    <t>Tarjeta Débito</t>
+  </si>
+  <si>
+    <t>Postgiro</t>
+  </si>
+  <si>
+    <t>Telex estándar bancario francés</t>
+  </si>
+  <si>
+    <t>Pago comercial urgente</t>
+  </si>
+  <si>
+    <t>Pago Tesorería Urgente</t>
+  </si>
+  <si>
+    <t>Nota promisoria</t>
+  </si>
+  <si>
+    <t>Nota promisoria firmada por el acreedor</t>
+  </si>
+  <si>
+    <t>Nota promisoria firmada por el acreedor, avalada por el banco</t>
+  </si>
+  <si>
+    <t>Nota promisoria firmada por el acreedor, avalada por un tercero</t>
+  </si>
+  <si>
+    <t>Nota promisoria firmada pro el banco</t>
+  </si>
+  <si>
+    <t>Nota promisoria firmada por un banco avalada por otro banco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nota promisoria firmada </t>
+  </si>
+  <si>
+    <t>Nota promisoria firmada por un tercero avalada por un banco</t>
+  </si>
+  <si>
+    <t>Retiro de nota por el por el acreedor</t>
+  </si>
+  <si>
+    <t>Retiro de nota por el por el acreedor sobre un banco</t>
+  </si>
+  <si>
+    <t>Retiro de nota por el acreedor, avalada por otro banco</t>
+  </si>
+  <si>
+    <t>Retiro de nota por el acreedor, sobre un banco avalada por un tercero</t>
+  </si>
+  <si>
+    <t>Retiro de una nota por el acreedor sobre un tercero</t>
+  </si>
+  <si>
+    <t>Retiro de una nota por el acreedor sobre un tercero avalada por un banco</t>
+  </si>
+  <si>
+    <t>Nota bancaria tranferible</t>
+  </si>
+  <si>
+    <t>Cheque local traferible</t>
+  </si>
+  <si>
+    <t>Giro referenciado</t>
+  </si>
+  <si>
+    <t>Giro urgente</t>
+  </si>
+  <si>
+    <t>Giro formato abierto</t>
+  </si>
+  <si>
+    <t>Método de pago solicitado no usuado</t>
+  </si>
+  <si>
+    <t>Clearing entre partners</t>
+  </si>
+  <si>
+    <t>Acuerdo mutuo</t>
+  </si>
+  <si>
+    <t>id_impuesto</t>
+  </si>
+  <si>
+    <t>monto_impuesto</t>
+  </si>
+  <si>
+    <t>porcentaje_impuesto</t>
+  </si>
+  <si>
+    <t>base_impuesto</t>
+  </si>
+  <si>
+    <t>id_impuesto_linea</t>
+  </si>
+  <si>
+    <t>monto_impuesto_linea</t>
+  </si>
+  <si>
+    <t>porcentaje_impuesto_linea</t>
+  </si>
+  <si>
+    <t>base_impuesto_linea</t>
+  </si>
+  <si>
+    <t>indicador_cargo</t>
+  </si>
+  <si>
+    <t>razon_descuento</t>
+  </si>
+  <si>
+    <t>monto_descuento</t>
+  </si>
+  <si>
+    <t>base_descuento</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>DESCUENTO</t>
+  </si>
+  <si>
     <t>227490.00</t>
   </si>
   <si>
-    <t>0.00</t>
-  </si>
-  <si>
-    <t>FUNDACION CLINICA NELSON MANDELA, Amor por servir</t>
-  </si>
-  <si>
-    <t>Calle 102 No. 24a 15, Barrio Compartir, Cali, Valle del Cauca - 602 389 9301 - www.ipsnelsonmandela.com</t>
-  </si>
-  <si>
-    <t>CALLE 102 No. 24A-15</t>
-  </si>
-  <si>
-    <t>18760000001</t>
-  </si>
-  <si>
-    <t>SETP</t>
-  </si>
-  <si>
     <t>PRUEBA1</t>
   </si>
   <si>
-    <t>PRUEBA2</t>
+    <t>AF-0000500-85-XX-001,4,A89008003,OBANDO,LONDOÑO,ALEXANDER,,1,7,5,A12345;604567;AX-2345,RNA3D345;664FF04567;ARXXX-2765345,RN6645G-345;6-064XX54FF04567;XXX-2-OO-987D65345,1000-2021-0005698,1045-2FG01-0567228,3300.00,5800.00,105000.00,225000.00%AF-0000500-85-XX-001,4,A41946692,CARDONA,VILLADA,ELIZABETH,,1,7,5,A12345;604567;AX-2345,RNA3D345;664FF04567;ARXXX-2765345,RN6645G-345;6-064XX54FF04567;XXX-2-OO-987D65345,1000-2021-0005698,1045-2FG01-0567228,3300.00,5800.00,105000.00,225000.00</t>
+  </si>
+  <si>
+    <t>AF-0000500-85-XX-001,4,A41946692,CARDONA,VILLADA,ELIZABETH,,1,7,5,A12345;604567;AX-2345,RNA3D345;664FF04567;ARXXX-2765345,RN6645G-345;6-064XX54FF04567;XXX-2-OO-987D65345,1000-2021-0005698,1045-2FG01-0567228,3300.00,5800.00,105000.00,225000.00</t>
   </si>
   <si>
     <t>682470.00</t>
   </si>
   <si>
-    <t>300000.00</t>
-  </si>
-  <si>
-    <t>AF-0000500-85-XX-001,4,A89008003,OBANDO,LONDOÑO,ALEXANDER,,1,7,5,A12345;604567;AX-2345,RNA3D345;664FF04567;ARXXX-2765345,RN6645G-345;6-064XX54FF04567;XXX-2-OO-987D65345,1000-2021-0005698,1045-2FG01-0567228,3300.00,5800.00,105000.00,225000.00</t>
-  </si>
-  <si>
-    <t>AF-0000500-85-XX-001,4,A41946692,CARDONA,VILLADA,ELIZABETH,,1,7,5,A12345;604567;AX-2345,RNA3D345;664FF04567;ARXXX-2765345,RN6645G-345;6-064XX54FF04567;XXX-2-OO-987D65345,1000-2021-0005698,1045-2FG01-0567228,3300.00,5800.00,105000.00,225000.00</t>
-  </si>
-  <si>
-    <t>AF-0000500-85-XX-001,4,A89008003,OBANDO,LONDOÑO,ALEXANDER,,1,7,5,A12345;604567;AX-2345,RNA3D345;664FF04567;ARXXX-2765345,RN6645G-345;6-064XX54FF04567;XXX-2-OO-987D65345,1000-2021-0005698,1045-2FG01-0567228,3300.00,5800.00,105000.00,225000.00%AF-0000500-85-XX-001,4,A41946692,CARDONA,VILLADA,ELIZABETH,,1,7,5,A12345;604567;AX-2345,RNA3D345;664FF04567;ARXXX-2765345,RN6645G-345;6-064XX54FF04567;XXX-2-OO-987D65345,1000-2021-0005698,1045-2FG01-0567228,3300.00,5800.00,105000.00,225000.00</t>
-  </si>
-  <si>
-    <t>numero</t>
-  </si>
-  <si>
-    <t>fecha</t>
-  </si>
-  <si>
-    <t>hora</t>
-  </si>
-  <si>
-    <t>numero_resolucion</t>
-  </si>
-  <si>
-    <t>prefijo</t>
-  </si>
-  <si>
-    <t>nombre_establecimiento</t>
-  </si>
-  <si>
-    <t>direccion_establecimiento</t>
-  </si>
-  <si>
-    <t>telefono_establecimiento</t>
-  </si>
-  <si>
-    <t>municipio_establecimiento</t>
-  </si>
-  <si>
-    <t>email_establecimiento</t>
-  </si>
-  <si>
-    <t>idetificacion_cliente</t>
-  </si>
-  <si>
-    <t>id_forma_pago</t>
-  </si>
-  <si>
-    <t>id_metodo_pago</t>
-  </si>
-  <si>
-    <t>fecha_vencimiento</t>
-  </si>
-  <si>
-    <t>plazo_dias</t>
-  </si>
-  <si>
-    <t>total_impuestos_incl</t>
-  </si>
-  <si>
-    <t>total_descuentos</t>
-  </si>
-  <si>
-    <t>total_cargos</t>
-  </si>
-  <si>
-    <t>total_pagado</t>
-  </si>
-  <si>
-    <t>cantidad_linea</t>
-  </si>
-  <si>
-    <t>base_impuestos_linea</t>
-  </si>
-  <si>
-    <t>codigo_linea</t>
-  </si>
-  <si>
-    <t>precio_venta</t>
-  </si>
-  <si>
-    <t>nota_cabecera</t>
-  </si>
-  <si>
-    <t>nota_pie</t>
-  </si>
-  <si>
-    <t>notas_factura</t>
-  </si>
-  <si>
-    <t>fecha_inicial_perido_facturado</t>
-  </si>
-  <si>
-    <t>fecha_final_perido_facturado</t>
-  </si>
-  <si>
-    <t>informacion_usuarios_sector_salud</t>
-  </si>
-  <si>
-    <t>total_base_impuestos</t>
-  </si>
-  <si>
-    <t>total_valor_bruto</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>Contado</t>
-  </si>
-  <si>
-    <t>Crédito</t>
-  </si>
-  <si>
-    <t>Instrumento no definido</t>
-  </si>
-  <si>
-    <t>Crédito ACH</t>
-  </si>
-  <si>
-    <t>Débito ACH</t>
-  </si>
-  <si>
-    <t>Reversión débito de demanda ACH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reversión crédito de demanda ACH </t>
-  </si>
-  <si>
-    <t>Crédito de demanda ACH</t>
-  </si>
-  <si>
-    <t>Débito de demanda ACH</t>
-  </si>
-  <si>
-    <t>Mantener</t>
-  </si>
-  <si>
-    <t>Clearing Nacional o Regional</t>
-  </si>
-  <si>
-    <t>Efectivo</t>
-  </si>
-  <si>
-    <t>Reversión Crédito Ahorro</t>
-  </si>
-  <si>
-    <t>Reversión Débito Ahorro</t>
-  </si>
-  <si>
-    <t>Crédito Ahorro</t>
-  </si>
-  <si>
-    <t>Débito Ahorro</t>
-  </si>
-  <si>
-    <t>Bookentry Crédito</t>
-  </si>
-  <si>
-    <t>Bookentry Débito</t>
-  </si>
-  <si>
-    <t>Concentración de la demanda en efectivo /Desembolso Crédito (CCD)</t>
-  </si>
-  <si>
-    <t>Concentración de la demanda en efectivo / Desembolso (CCD) débito</t>
-  </si>
-  <si>
-    <t>Crédito Pago negocio corporativo (CTP)</t>
-  </si>
-  <si>
-    <t>Cheque</t>
-  </si>
-  <si>
-    <t>Poyecto bancario</t>
-  </si>
-  <si>
-    <t>Proyecto bancario certificado</t>
-  </si>
-  <si>
-    <t>Cheque bancario</t>
-  </si>
-  <si>
-    <t>Nota cambiaria esperando aceptación</t>
-  </si>
-  <si>
-    <t>Cheque certificado</t>
-  </si>
-  <si>
-    <t>Cheque Local</t>
-  </si>
-  <si>
-    <t>Débito Pago Neogcio Corporativo (CTP)</t>
-  </si>
-  <si>
-    <t>Crédito Negocio Intercambio Corporativo (CTX)</t>
-  </si>
-  <si>
-    <t>Débito Negocio Intercambio Corporativo (CTX)</t>
-  </si>
-  <si>
-    <t>Transferecia Crédito</t>
-  </si>
-  <si>
-    <t>Transferencia Débito</t>
-  </si>
-  <si>
-    <t>Concentración Efectivo / Desembolso Crédito plus (CCD+)</t>
-  </si>
-  <si>
-    <t>Concentración Efectivo / Desembolso Débito plus (CCD+)</t>
-  </si>
-  <si>
-    <t>Pago y depósito pre acordado (PPD)</t>
-  </si>
-  <si>
-    <t>Concentración efectivo ahorros / Desembolso Crédito (CCD)</t>
-  </si>
-  <si>
-    <t>Concentración efectivo ahorros / Desembolso Drédito (CCD)</t>
-  </si>
-  <si>
-    <t>Pago Negocio Corporativo Ahorros Crédito (CTP)</t>
-  </si>
-  <si>
-    <t>Pago Neogcio Corporativo Ahorros Débito (CTP)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Concentración efectivo/Desembolso Crédito plus (CCD+) </t>
-  </si>
-  <si>
-    <t>Consiganción bancaria</t>
-  </si>
-  <si>
-    <t>Concentración efectivo / Desembolso Débito plus (CCD+)</t>
-  </si>
-  <si>
-    <t>Nota cambiaria</t>
-  </si>
-  <si>
-    <t>Transferencia Crédito Bancario</t>
-  </si>
-  <si>
-    <t>Transferencia Débito Interbancario</t>
-  </si>
-  <si>
-    <t>Transferencia Débito Bancaria</t>
-  </si>
-  <si>
-    <t>Tarjeta Crédito</t>
-  </si>
-  <si>
-    <t>Tarjeta Débito</t>
-  </si>
-  <si>
-    <t>Postgiro</t>
-  </si>
-  <si>
-    <t>Telex estándar bancario francés</t>
-  </si>
-  <si>
-    <t>Pago comercial urgente</t>
-  </si>
-  <si>
-    <t>Pago Tesorería Urgente</t>
-  </si>
-  <si>
-    <t>Nota promisoria</t>
-  </si>
-  <si>
-    <t>Nota promisoria firmada por el acreedor</t>
-  </si>
-  <si>
-    <t>Nota promisoria firmada por el acreedor, avalada por el banco</t>
-  </si>
-  <si>
-    <t>Nota promisoria firmada por el acreedor, avalada por un tercero</t>
-  </si>
-  <si>
-    <t>Nota promisoria firmada pro el banco</t>
-  </si>
-  <si>
-    <t>Nota promisoria firmada por un banco avalada por otro banco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nota promisoria firmada </t>
-  </si>
-  <si>
-    <t>Nota promisoria firmada por un tercero avalada por un banco</t>
-  </si>
-  <si>
-    <t>Retiro de nota por el por el acreedor</t>
-  </si>
-  <si>
-    <t>Retiro de nota por el por el acreedor sobre un banco</t>
-  </si>
-  <si>
-    <t>Retiro de nota por el acreedor, avalada por otro banco</t>
-  </si>
-  <si>
-    <t>Retiro de nota por el acreedor, sobre un banco avalada por un tercero</t>
-  </si>
-  <si>
-    <t>Retiro de una nota por el acreedor sobre un tercero</t>
-  </si>
-  <si>
-    <t>Retiro de una nota por el acreedor sobre un tercero avalada por un banco</t>
-  </si>
-  <si>
-    <t>Nota bancaria tranferible</t>
-  </si>
-  <si>
-    <t>Cheque local traferible</t>
-  </si>
-  <si>
-    <t>Giro referenciado</t>
-  </si>
-  <si>
-    <t>Giro urgente</t>
-  </si>
-  <si>
-    <t>Giro formato abierto</t>
-  </si>
-  <si>
-    <t>Método de pago solicitado no usuado</t>
-  </si>
-  <si>
-    <t>Clearing entre partners</t>
-  </si>
-  <si>
-    <t>Acuerdo mutuo</t>
-  </si>
-  <si>
-    <t>991500178</t>
-  </si>
-  <si>
-    <t>991500179</t>
-  </si>
-  <si>
-    <t>991500180</t>
-  </si>
-  <si>
-    <t>991500181</t>
-  </si>
-  <si>
-    <t>991500182</t>
-  </si>
-  <si>
-    <t>991500183</t>
+    <t>994500046</t>
+  </si>
+  <si>
+    <t>994500047</t>
+  </si>
+  <si>
+    <t>994500048</t>
+  </si>
+  <si>
+    <t>994500049</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="[h]:mm:ss;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1239,6 +1274,14 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1260,12 +1303,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1326,7 +1370,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1361,7 +1405,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1538,21 +1582,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AQ16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AE6" sqref="AE6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AQ2" sqref="AQ2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
@@ -1571,7 +1615,7 @@
     <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="21" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.140625" customWidth="1"/>
     <col min="19" max="19" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="20" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -1585,124 +1629,171 @@
     <col min="29" max="29" width="28.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="27.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="32.7109375" customWidth="1"/>
+    <col min="32" max="32" width="12.7109375" customWidth="1"/>
+    <col min="33" max="33" width="17.28515625" customWidth="1"/>
+    <col min="34" max="34" width="20.140625" customWidth="1"/>
+    <col min="35" max="35" width="16" customWidth="1"/>
+    <col min="36" max="36" width="20" customWidth="1"/>
+    <col min="37" max="37" width="22.42578125" customWidth="1"/>
+    <col min="38" max="38" width="25.7109375" customWidth="1"/>
+    <col min="39" max="39" width="21.5703125" customWidth="1"/>
+    <col min="40" max="40" width="17.42578125" customWidth="1"/>
+    <col min="41" max="42" width="17.140625" customWidth="1"/>
+    <col min="43" max="43" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="J1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="K1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="L1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="M1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" t="s">
+      <c r="N1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H1" t="s">
+      <c r="O1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" t="s">
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" t="s">
+      <c r="S1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" t="s">
+      <c r="T1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" t="s">
+      <c r="U1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" t="s">
+      <c r="V1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="W1" t="s">
         <v>30</v>
       </c>
-      <c r="O1" t="s">
+      <c r="X1" t="s">
         <v>31</v>
       </c>
-      <c r="P1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>46</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="Y1" t="s">
         <v>32</v>
       </c>
-      <c r="S1" t="s">
+      <c r="Z1" t="s">
         <v>33</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AA1" t="s">
         <v>34</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AB1" t="s">
         <v>35</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AC1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AD1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AE1" t="s">
         <v>38</v>
       </c>
-      <c r="Y1" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31">
+      <c r="AF1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="B2" s="3">
-        <v>45180</v>
+        <v>45820</v>
       </c>
       <c r="C2" s="4">
-        <v>0.69513888888888886</v>
+        <v>0.69652777777777775</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H2">
         <v>3899301</v>
@@ -1717,87 +1808,114 @@
         <v>89008003</v>
       </c>
       <c r="L2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="M2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="N2" s="3">
-        <v>45210</v>
+        <v>45850</v>
       </c>
       <c r="O2">
         <v>30</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2">
+        <v>769500</v>
+      </c>
+      <c r="Q2">
+        <v>950000</v>
+      </c>
+      <c r="R2">
+        <v>950000</v>
+      </c>
+      <c r="S2" t="s">
         <v>3</v>
       </c>
-      <c r="Q2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>3</v>
       </c>
-      <c r="S2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T2" t="s">
-        <v>4</v>
-      </c>
-      <c r="U2" t="s">
-        <v>3</v>
+      <c r="U2">
+        <v>950000</v>
       </c>
       <c r="V2">
         <v>1</v>
       </c>
-      <c r="W2" t="s">
-        <v>3</v>
+      <c r="W2">
+        <v>769500</v>
       </c>
       <c r="X2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="Y2">
+        <v>1000000</v>
       </c>
       <c r="Z2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA2" t="s">
         <v>5</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>6</v>
       </c>
       <c r="AB2" t="s">
         <v>0</v>
       </c>
-      <c r="AC2" s="3">
-        <v>45108</v>
-      </c>
-      <c r="AD2" s="3">
-        <v>45138</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31">
+      <c r="AF2">
+        <v>1</v>
+      </c>
+      <c r="AG2">
+        <v>180500</v>
+      </c>
+      <c r="AH2">
+        <v>19</v>
+      </c>
+      <c r="AI2">
+        <v>950000</v>
+      </c>
+      <c r="AJ2">
+        <v>1</v>
+      </c>
+      <c r="AK2">
+        <v>180500</v>
+      </c>
+      <c r="AL2">
+        <v>19</v>
+      </c>
+      <c r="AM2">
+        <v>950000</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AP2">
+        <v>50000</v>
+      </c>
+      <c r="AQ2">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="B3" s="3">
-        <v>45180</v>
+        <v>45820</v>
       </c>
       <c r="C3" s="4">
-        <v>0.6958333333333333</v>
+        <v>0.69513888888888886</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
         <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H3">
         <v>3899301</v>
@@ -1812,52 +1930,52 @@
         <v>89008003</v>
       </c>
       <c r="L3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M3">
-        <v>47</v>
+        <v>44</v>
+      </c>
+      <c r="M3" t="s">
+        <v>45</v>
       </c>
       <c r="N3" s="3">
-        <v>45180</v>
+        <v>45210</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="P3" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q3" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" t="s">
-        <v>4</v>
-      </c>
       <c r="R3" t="s">
+        <v>132</v>
+      </c>
+      <c r="S3" t="s">
         <v>3</v>
       </c>
-      <c r="S3" t="s">
-        <v>4</v>
-      </c>
       <c r="T3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U3" t="s">
-        <v>3</v>
+        <v>132</v>
       </c>
       <c r="V3">
         <v>1</v>
       </c>
       <c r="W3" t="s">
-        <v>3</v>
+        <v>132</v>
       </c>
       <c r="X3" t="s">
-        <v>11</v>
+        <v>133</v>
       </c>
       <c r="Y3" t="s">
-        <v>3</v>
+        <v>132</v>
       </c>
       <c r="Z3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA3" t="s">
         <v>5</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>6</v>
       </c>
       <c r="AB3" t="s">
         <v>0</v>
@@ -1869,30 +1987,30 @@
         <v>45138</v>
       </c>
       <c r="AE3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="B4" s="3">
-        <v>45180</v>
+        <v>45820</v>
       </c>
       <c r="C4" s="4">
-        <v>0.69652777777777775</v>
+        <v>0.6958333333333333</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
         <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
       </c>
       <c r="F4" t="s">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H4">
         <v>3899301</v>
@@ -1906,79 +2024,88 @@
       <c r="K4">
         <v>89008003</v>
       </c>
-      <c r="L4">
-        <v>2</v>
-      </c>
-      <c r="M4" t="s">
-        <v>57</v>
+      <c r="L4" t="s">
+        <v>43</v>
+      </c>
+      <c r="M4">
+        <v>47</v>
       </c>
       <c r="N4" s="3">
-        <v>45210</v>
+        <v>45180</v>
       </c>
       <c r="O4">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>13</v>
+        <v>132</v>
       </c>
       <c r="Q4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R4" t="s">
+        <v>132</v>
+      </c>
+      <c r="S4" t="s">
         <v>3</v>
       </c>
-      <c r="S4" t="s">
-        <v>4</v>
-      </c>
       <c r="T4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U4" t="s">
-        <v>3</v>
+        <v>132</v>
       </c>
       <c r="V4">
         <v>1</v>
       </c>
       <c r="W4" t="s">
-        <v>3</v>
+        <v>132</v>
       </c>
       <c r="X4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="Y4" t="s">
-        <v>3</v>
+        <v>132</v>
       </c>
       <c r="Z4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA4" t="s">
         <v>5</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>6</v>
       </c>
       <c r="AB4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:31">
+      <c r="AC4" s="3">
+        <v>45108</v>
+      </c>
+      <c r="AD4" s="3">
+        <v>45138</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="B5" s="3">
-        <v>45180</v>
+        <v>45820</v>
       </c>
       <c r="C5" s="4">
-        <v>0.6972222222222223</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
         <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
       </c>
       <c r="F5" t="s">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H5">
         <v>3899301</v>
@@ -2005,40 +2132,40 @@
         <v>30</v>
       </c>
       <c r="P5" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q5" t="s">
         <v>3</v>
       </c>
-      <c r="Q5" t="s">
-        <v>4</v>
-      </c>
       <c r="R5" t="s">
+        <v>136</v>
+      </c>
+      <c r="S5" t="s">
         <v>3</v>
       </c>
-      <c r="S5" t="s">
-        <v>4</v>
-      </c>
       <c r="T5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U5" t="s">
-        <v>3</v>
+        <v>136</v>
       </c>
       <c r="V5">
         <v>1</v>
       </c>
       <c r="W5" t="s">
-        <v>3</v>
+        <v>132</v>
       </c>
       <c r="X5" t="s">
-        <v>10</v>
+        <v>133</v>
       </c>
       <c r="Y5" t="s">
-        <v>3</v>
+        <v>132</v>
       </c>
       <c r="Z5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA5" t="s">
         <v>5</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>6</v>
       </c>
       <c r="AB5" t="s">
         <v>0</v>
@@ -2049,31 +2176,28 @@
       <c r="AD5" s="3">
         <v>45138</v>
       </c>
-      <c r="AE5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31">
+    </row>
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="B6" s="3">
-        <v>45180</v>
+        <v>45820</v>
       </c>
       <c r="C6" s="4">
         <v>0.69791666666666663</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
         <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
       </c>
       <c r="F6" t="s">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H6">
         <v>3899301</v>
@@ -2100,40 +2224,40 @@
         <v>30</v>
       </c>
       <c r="P6" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
       <c r="Q6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R6" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
       <c r="S6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U6" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
       <c r="V6">
         <v>1</v>
       </c>
       <c r="W6" t="s">
-        <v>3</v>
+        <v>132</v>
       </c>
       <c r="X6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Y6" t="s">
-        <v>3</v>
+        <v>132</v>
       </c>
       <c r="Z6" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA6" t="s">
         <v>5</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>6</v>
       </c>
       <c r="AB6" t="s">
         <v>0</v>
@@ -2145,27 +2269,27 @@
         <v>45138</v>
       </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="B7" s="3">
-        <v>45180</v>
+        <v>45820</v>
       </c>
       <c r="C7" s="4">
         <v>0.69791666666666663</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
         <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
       </c>
       <c r="F7" t="s">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H7">
         <v>3899301</v>
@@ -2192,40 +2316,40 @@
         <v>30</v>
       </c>
       <c r="P7" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
       <c r="Q7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R7" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
       <c r="S7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U7" t="s">
-        <v>12</v>
+        <v>136</v>
       </c>
       <c r="V7">
         <v>1</v>
       </c>
       <c r="W7" t="s">
-        <v>3</v>
+        <v>132</v>
       </c>
       <c r="X7" t="s">
-        <v>11</v>
+        <v>133</v>
       </c>
       <c r="Y7" t="s">
-        <v>3</v>
+        <v>132</v>
       </c>
       <c r="Z7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA7" t="s">
         <v>5</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>6</v>
       </c>
       <c r="AB7" t="s">
         <v>0</v>
@@ -2237,382 +2361,20 @@
         <v>45138</v>
       </c>
     </row>
-    <row r="8" spans="1:31">
-      <c r="A8" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B8" s="3">
-        <v>45180</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0.69791666666666663</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8">
-        <v>3899301</v>
-      </c>
-      <c r="I8">
-        <v>1006</v>
-      </c>
-      <c r="J8" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8">
-        <v>89008003</v>
-      </c>
-      <c r="L8">
-        <v>2</v>
-      </c>
-      <c r="M8">
-        <v>47</v>
-      </c>
-      <c r="N8" s="3">
-        <v>45210</v>
-      </c>
-      <c r="O8">
-        <v>30</v>
-      </c>
-      <c r="P8" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>4</v>
-      </c>
-      <c r="R8" t="s">
-        <v>12</v>
-      </c>
-      <c r="S8" t="s">
-        <v>4</v>
-      </c>
-      <c r="T8" t="s">
-        <v>4</v>
-      </c>
-      <c r="U8" t="s">
-        <v>12</v>
-      </c>
-      <c r="V8">
-        <v>1</v>
-      </c>
-      <c r="W8" t="s">
-        <v>3</v>
-      </c>
-      <c r="X8" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z8" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="3">
-        <v>45108</v>
-      </c>
-      <c r="AD8" s="3">
-        <v>45138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31">
-      <c r="A9" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B9" s="3">
-        <v>45180</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0.69791666666666663</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9">
-        <v>3899301</v>
-      </c>
-      <c r="I9">
-        <v>1006</v>
-      </c>
-      <c r="J9" t="s">
-        <v>2</v>
-      </c>
-      <c r="K9">
-        <v>89008003</v>
-      </c>
-      <c r="L9" t="s">
-        <v>50</v>
-      </c>
-      <c r="M9">
-        <v>10</v>
-      </c>
-      <c r="N9" s="3">
-        <v>45180</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>4</v>
-      </c>
-      <c r="R9" t="s">
-        <v>12</v>
-      </c>
-      <c r="S9" t="s">
-        <v>4</v>
-      </c>
-      <c r="T9" t="s">
-        <v>4</v>
-      </c>
-      <c r="U9" t="s">
-        <v>12</v>
-      </c>
-      <c r="V9">
-        <v>1</v>
-      </c>
-      <c r="W9" t="s">
-        <v>3</v>
-      </c>
-      <c r="X9" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="3">
-        <v>45108</v>
-      </c>
-      <c r="AD9" s="3">
-        <v>45138</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31">
-      <c r="A10" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B10" s="3">
-        <v>45180</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0.69791666666666663</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10">
-        <v>3899301</v>
-      </c>
-      <c r="I10">
-        <v>1006</v>
-      </c>
-      <c r="J10" t="s">
-        <v>2</v>
-      </c>
-      <c r="K10">
-        <v>89008003</v>
-      </c>
-      <c r="L10" t="s">
-        <v>50</v>
-      </c>
-      <c r="M10">
-        <v>10</v>
-      </c>
-      <c r="N10" s="3">
-        <v>45180</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>4</v>
-      </c>
-      <c r="R10" t="s">
-        <v>12</v>
-      </c>
-      <c r="S10" t="s">
-        <v>4</v>
-      </c>
-      <c r="T10" t="s">
-        <v>4</v>
-      </c>
-      <c r="U10" t="s">
-        <v>12</v>
-      </c>
-      <c r="V10">
-        <v>1</v>
-      </c>
-      <c r="W10" t="s">
-        <v>3</v>
-      </c>
-      <c r="X10" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="3">
-        <v>45108</v>
-      </c>
-      <c r="AD10" s="3">
-        <v>45138</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31">
-      <c r="A11" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11" s="3">
-        <v>45180</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0.69791666666666663</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11">
-        <v>3899301</v>
-      </c>
-      <c r="I11">
-        <v>1006</v>
-      </c>
-      <c r="J11" t="s">
-        <v>2</v>
-      </c>
-      <c r="K11">
-        <v>89008003</v>
-      </c>
-      <c r="L11" t="s">
-        <v>50</v>
-      </c>
-      <c r="M11">
-        <v>10</v>
-      </c>
-      <c r="N11" s="3">
-        <v>45180</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>4</v>
-      </c>
-      <c r="R11" t="s">
-        <v>12</v>
-      </c>
-      <c r="S11" t="s">
-        <v>4</v>
-      </c>
-      <c r="T11" t="s">
-        <v>4</v>
-      </c>
-      <c r="U11" t="s">
-        <v>12</v>
-      </c>
-      <c r="V11">
-        <v>1</v>
-      </c>
-      <c r="W11" t="s">
-        <v>3</v>
-      </c>
-      <c r="X11" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y11" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="3">
-        <v>45108</v>
-      </c>
-      <c r="AD11" s="3">
-        <v>45138</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>16</v>
-      </c>
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+    </row>
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="W16" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -2630,41 +2392,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2673,625 +2435,625 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>